<commit_message>
#1152 initial approach with sets and hashmap setup
</commit_message>
<xml_diff>
--- a/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
+++ b/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\1152. Analyze User Website Visit Pattern\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB7C676-86CC-4A2B-828F-9D350897F58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -32,6 +32,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+  <si>
+    <t>joe</t>
+  </si>
+  <si>
+    <t>james</t>
+  </si>
+  <si>
+    <t>mary</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>career</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>maps</t>
+  </si>
+  <si>
+    <t>highscore</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,17 +419,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="E4:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2</v>
+      </c>
+      <c r="V4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1">
+        <v>8</v>
+      </c>
+      <c r="M7" s="1">
+        <v>9</v>
+      </c>
+      <c r="N7" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
#1152 at realization that patterns can consist of non-consecutive candidates
</commit_message>
<xml_diff>
--- a/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
+++ b/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\1152. Analyze User Website Visit Pattern\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB7C676-86CC-4A2B-828F-9D350897F58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C203F1-42A0-4079-BF9A-AD162E0379D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
   <si>
     <t>joe</t>
   </si>
@@ -65,6 +65,78 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>bcd</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>ce</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>bf</t>
+  </si>
+  <si>
+    <t>cf</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>ef</t>
   </si>
 </sst>
 </file>
@@ -419,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="E4:AC8"/>
+  <dimension ref="E4:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="V40" sqref="V40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -430,7 +502,7 @@
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T4" s="1">
         <v>1</v>
       </c>
@@ -447,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q5" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>1</v>
       </c>
@@ -537,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="5:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
@@ -567,6 +639,643 @@
       </c>
       <c r="N8" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="5:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB37" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y41" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y42" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y43" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y45" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y46" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y47" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="25:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y49" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="25:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="25:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y52" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1152 non-consecutive pattern correction attempt
</commit_message>
<xml_diff>
--- a/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
+++ b/1152. Analyze User Website Visit Pattern/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\1152. Analyze User Website Visit Pattern\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C203F1-42A0-4079-BF9A-AD162E0379D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF878104-39E0-4D42-88D8-185C49E50388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="-23955" yWindow="1650" windowWidth="18315" windowHeight="11385" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="34">
   <si>
     <t>joe</t>
   </si>
@@ -494,7 +494,7 @@
   <dimension ref="E4:AG52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V40" sqref="V40"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -839,7 +839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q17" s="1" t="s">
         <v>11</v>
       </c>
@@ -856,7 +856,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q20" s="1" t="s">
         <v>11</v>
       </c>
@@ -891,7 +891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P21" s="1" t="s">
         <v>11</v>
       </c>
@@ -932,7 +932,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P22" s="1" t="s">
         <v>12</v>
       </c>
@@ -967,7 +967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P23" s="1" t="s">
         <v>13</v>
       </c>
@@ -996,7 +996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AF26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1041,12 +1041,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="16:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AF27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AG27" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1">
+        <v>3</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="5:33" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="5:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>